<commit_message>
[Data] : correction datas
</commit_message>
<xml_diff>
--- a/src/main/resources/testFiles/suivi_check.xlsx
+++ b/src/main/resources/testFiles/suivi_check.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -103,14 +103,18 @@
   </si>
   <si>
     <t>uotap</t>
+  </si>
+  <si>
+    <t>8.92</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -161,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -184,12 +188,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -227,11 +240,8 @@
     <xf numFmtId="44" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,6 +252,9 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -249,6 +262,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -571,9 +592,9 @@
   </sheetPr>
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N11" sqref="N11:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -587,13 +608,13 @@
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
     <col min="8" max="8" width="7.42578125" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" customWidth="1"/>
-    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -630,12 +651,12 @@
       <c r="L1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="40"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N1" s="33"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43437</v>
       </c>
@@ -666,20 +687,23 @@
         <f>(J2-INT(J2))*24</f>
         <v>8.9166666666666661</v>
       </c>
-      <c r="L2" s="12">
-        <f>K2-I2</f>
-        <v>-3.3333333333338544E-3</v>
-      </c>
-      <c r="M2" s="35">
+      <c r="L2" s="41">
+        <v>0</v>
+      </c>
+      <c r="M2" s="34">
         <f>SUM(K2:K3)</f>
         <v>10.083333333333332</v>
       </c>
-      <c r="N2" s="33">
+      <c r="N2" s="37">
         <f>IF(M2&gt;9,3.03,2.65)</f>
         <v>3.03</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O2" s="44">
+        <f>SUM(N2:N8)</f>
+        <v>11.74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43437</v>
       </c>
@@ -709,14 +733,18 @@
         <f t="shared" ref="K3:K22" si="0">(J3-INT(J3))*24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="41">
         <f t="shared" ref="L3:L21" si="1">K3-I3</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="M3" s="36"/>
-      <c r="N3" s="33"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M3" s="35"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="3">
+        <v>0.69791666666424135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43438</v>
       </c>
@@ -747,20 +775,21 @@
         <f t="shared" si="0"/>
         <v>11.083333333333334</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="41">
         <f t="shared" si="1"/>
         <v>2.163333333333334</v>
       </c>
-      <c r="M4" s="35">
+      <c r="M4" s="34">
         <f>SUM(K4:K5)</f>
         <v>12.416666666666668</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="37">
         <f>IF(M4&gt;9,3.03,2.65)</f>
         <v>3.03</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O4" s="43"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43438</v>
       </c>
@@ -790,14 +819,15 @@
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="41">
         <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="M5" s="36"/>
-      <c r="N5" s="33"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M5" s="35"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="43"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43440</v>
       </c>
@@ -828,20 +858,20 @@
         <f t="shared" si="0"/>
         <v>8.9166666666666661</v>
       </c>
-      <c r="L6" s="12">
-        <f t="shared" si="1"/>
-        <v>-3.3333333333338544E-3</v>
-      </c>
-      <c r="M6" s="35">
+      <c r="L6" s="41">
+        <v>0</v>
+      </c>
+      <c r="M6" s="34">
         <f>SUM(K6:K7)</f>
         <v>10.083333333333332</v>
       </c>
-      <c r="N6" s="33">
+      <c r="N6" s="37">
         <f>IF(M6&gt;9,3.03,2.65)</f>
         <v>3.03</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O6" s="43"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43440</v>
       </c>
@@ -871,14 +901,15 @@
         <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="41">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="M7" s="36"/>
-      <c r="N7" s="33"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="35"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="43"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43441</v>
       </c>
@@ -909,7 +940,7 @@
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -921,8 +952,9 @@
         <f>IF(M8&gt;9,3.03,2.65)</f>
         <v>2.65</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O8" s="43"/>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>43444</v>
       </c>
@@ -954,20 +986,23 @@
         <f t="shared" si="0"/>
         <v>8.9166666666666661</v>
       </c>
-      <c r="L9" s="13">
-        <f t="shared" si="1"/>
-        <v>-3.3333333333338544E-3</v>
+      <c r="L9" s="42">
+        <v>0</v>
       </c>
       <c r="M9" s="38">
         <f>SUM(K9:K10)</f>
         <v>10.083333333333332</v>
       </c>
-      <c r="N9" s="37">
+      <c r="N9" s="36">
         <f>IF(M9&gt;9,3.03,2.65)</f>
         <v>3.03</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O9" s="44">
+        <f>SUM(N9:N15)</f>
+        <v>11.74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>43444</v>
       </c>
@@ -999,14 +1034,15 @@
         <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="42">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="M10" s="39"/>
-      <c r="N10" s="37"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N10" s="36"/>
+      <c r="O10" s="44"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>43445</v>
       </c>
@@ -1038,20 +1074,21 @@
         <f t="shared" si="0"/>
         <v>11.083333333333334</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="42">
         <f t="shared" si="1"/>
         <v>2.0033333333333339</v>
       </c>
       <c r="M11" s="38">
         <f>SUM(K11:K12)</f>
-        <v>12.416666666666668</v>
-      </c>
-      <c r="N11" s="37">
+        <v>14.416666666666668</v>
+      </c>
+      <c r="N11" s="36">
         <f>IF(M11&gt;9,3.03,2.65)</f>
         <v>3.03</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O11" s="44"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>43445</v>
       </c>
@@ -1080,21 +1117,22 @@
         <v>0</v>
       </c>
       <c r="J12" s="10" t="str">
-        <f>TEXT($E12-$D12,"h:mm")</f>
-        <v>1:20</v>
+        <f>TEXT($E12-$D12 +( F12-P3),"h:mm")</f>
+        <v>3:20</v>
       </c>
       <c r="K12" s="13">
         <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="L12" s="13">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="L12" s="42">
         <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="M12" s="39"/>
-      <c r="N12" s="37"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N12" s="36"/>
+      <c r="O12" s="44"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>43447</v>
       </c>
@@ -1126,20 +1164,23 @@
         <f t="shared" si="0"/>
         <v>8.9166666666666661</v>
       </c>
-      <c r="L13" s="13">
-        <f t="shared" si="1"/>
-        <v>-3.3333333333338544E-3</v>
+      <c r="L13" s="42">
+        <v>0</v>
       </c>
       <c r="M13" s="38">
         <f>SUM(K13:K14)</f>
         <v>10.083333333333332</v>
       </c>
-      <c r="N13" s="37">
+      <c r="N13" s="36">
         <f>IF(M13&gt;9,3.03,2.65)</f>
         <v>3.03</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O13" s="44"/>
+      <c r="P13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>43447</v>
       </c>
@@ -1171,14 +1212,15 @@
         <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="42">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="M14" s="39"/>
-      <c r="N14" s="37"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N14" s="36"/>
+      <c r="O14" s="44"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>43448</v>
       </c>
@@ -1210,7 +1252,7 @@
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="42">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1222,8 +1264,12 @@
         <f>IF(M15&gt;9,3.03,2.65)</f>
         <v>2.65</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O15" s="44"/>
+      <c r="P15">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43451</v>
       </c>
@@ -1254,17 +1300,21 @@
         <f t="shared" si="0"/>
         <v>10.916666666666666</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="41">
         <f t="shared" si="1"/>
         <v>1.9966666666666661</v>
       </c>
-      <c r="M16" s="35">
+      <c r="M16" s="34">
         <f>SUM(K16:K17)</f>
         <v>12.083333333333332</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N16" s="37">
         <f>IF(M16&gt;9,3.03,2.65)</f>
         <v>3.03</v>
+      </c>
+      <c r="O16" s="44">
+        <f>SUM(N16:N22)</f>
+        <v>11.74</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1297,12 +1347,13 @@
         <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="41">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="M17" s="36"/>
-      <c r="N17" s="33"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="43"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1335,18 +1386,19 @@
         <f t="shared" si="0"/>
         <v>9.5833333333333339</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="41">
         <f t="shared" si="1"/>
         <v>0.663333333333334</v>
       </c>
-      <c r="M18" s="35">
+      <c r="M18" s="34">
         <f>SUM(K18:K19)</f>
         <v>11.416666666666668</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N18" s="37">
         <f>IF(M18&gt;9,3.03,2.65)</f>
         <v>3.03</v>
       </c>
+      <c r="O18" s="43"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1378,12 +1430,13 @@
         <f t="shared" si="0"/>
         <v>1.8333333333333335</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="41">
         <f t="shared" si="1"/>
         <v>1.8333333333333335</v>
       </c>
-      <c r="M19" s="36"/>
-      <c r="N19" s="33"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="43"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1416,18 +1469,18 @@
         <f t="shared" si="0"/>
         <v>8.9166666666666661</v>
       </c>
-      <c r="L20" s="12">
-        <f t="shared" si="1"/>
-        <v>-3.3333333333338544E-3</v>
-      </c>
-      <c r="M20" s="35">
+      <c r="L20" s="41">
+        <v>0</v>
+      </c>
+      <c r="M20" s="34">
         <f>SUM(K20:K21)</f>
         <v>10.083333333333332</v>
       </c>
-      <c r="N20" s="33">
+      <c r="N20" s="37">
         <f>IF(M20&gt;9,3.03,2.65)</f>
         <v>3.03</v>
       </c>
+      <c r="O20" s="43"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1459,12 +1512,13 @@
         <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="41">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="M21" s="36"/>
-      <c r="N21" s="33"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="43"/>
     </row>
     <row r="22" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1497,7 +1551,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="41">
         <v>0</v>
       </c>
       <c r="M22" s="4">
@@ -1508,9 +1562,10 @@
         <f>IF(M22&gt;9,3.03,2.65)</f>
         <v>2.65</v>
       </c>
+      <c r="O22" s="43"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="40" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="6" t="s">
@@ -1527,12 +1582,12 @@
       </c>
       <c r="L24" s="14">
         <f>SUM(L16:L22,L2:L8)</f>
-        <v>12.646666666666667</v>
+        <v>12.656666666666668</v>
       </c>
       <c r="M24" s="6"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F25" s="34"/>
+      <c r="F25" s="40"/>
       <c r="H25" s="15" t="s">
         <v>6</v>
       </c>
@@ -1543,16 +1598,16 @@
       <c r="J25" s="23"/>
       <c r="K25" s="22">
         <f>SUM(K9:K15)</f>
-        <v>40.333333333333329</v>
+        <v>42.333333333333329</v>
       </c>
       <c r="L25" s="16">
         <f>SUM(L9:L15)</f>
-        <v>5.6633333333333331</v>
+        <v>7.6700000000000008</v>
       </c>
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F26" s="34" t="s">
+      <c r="F26" s="40" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="6" t="s">
@@ -1563,27 +1618,27 @@
       </c>
       <c r="L26" s="25">
         <f>L24*2.93</f>
-        <v>37.054733333333338</v>
+        <v>37.084033333333338</v>
       </c>
       <c r="N26" s="19">
-        <f>SUM(N2:N8,N16:N22)</f>
+        <f>SUM(O2,O16)</f>
         <v>23.48</v>
       </c>
       <c r="O26" s="28">
         <f>I26+L26</f>
-        <v>197.15473333333333</v>
+        <v>197.18403333333333</v>
       </c>
       <c r="P26" s="20">
         <f>O26*1.1</f>
-        <v>216.87020666666669</v>
+        <v>216.90243666666669</v>
       </c>
       <c r="Q26" s="28">
         <f>SUM(P26+G26+N26)</f>
-        <v>240.35020666666668</v>
+        <v>240.38243666666668</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F27" s="34"/>
+      <c r="F27" s="40"/>
       <c r="G27" s="19">
         <f>SUM(G9:G15)*1</f>
         <v>1</v>
@@ -1598,7 +1653,7 @@
       <c r="K27" s="10"/>
       <c r="L27" s="32">
         <f>L25*2.93</f>
-        <v>16.593566666666668</v>
+        <v>22.473100000000002</v>
       </c>
       <c r="M27" s="10"/>
       <c r="N27" s="18">
@@ -1607,15 +1662,15 @@
       </c>
       <c r="O27" s="29">
         <f>I27+L27</f>
-        <v>177.43356666666668</v>
+        <v>183.31310000000002</v>
       </c>
       <c r="P27" s="30">
         <f>O27*1.1</f>
-        <v>195.17692333333335</v>
+        <v>201.64441000000005</v>
       </c>
       <c r="Q27" s="29">
         <f>SUM(P27+G27+N27)</f>
-        <v>207.91692333333336</v>
+        <v>214.38441000000006</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1630,28 +1685,31 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N13:N14"/>
+  <mergeCells count="24">
+    <mergeCell ref="O2:O8"/>
+    <mergeCell ref="O16:O22"/>
+    <mergeCell ref="O9:O15"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="M20:M21"/>
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="N18:N19"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="M13:M14"/>
     <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N13:N14"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="M20:M21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>